<commit_message>
Validated validlogin script and created batchrunner
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14250" windowHeight="6165"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -410,7 +411,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A3:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>